<commit_message>
Commited automation scripts for "City and SubCity" masters
</commit_message>
<xml_diff>
--- a/src/main/resources/ExcelFiles/testdataKerchanshe.xlsx
+++ b/src/main/resources/ExcelFiles/testdataKerchanshe.xlsx
@@ -3,17 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1C4463E2-9F60-4C14-B0B1-654C40AECE85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\git\com.kerchanshe-buna\src\main\resources\ExcelFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB156C7-938A-4E21-9ED0-CDFED08B2876}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19770" windowHeight="5895" activeTab="2" xr2:uid="{1044F498-CD87-46B0-BBCE-0AF35426E927}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17772" windowHeight="7608" activeTab="3" xr2:uid="{1044F498-CD87-46B0-BBCE-0AF35426E927}"/>
   </bookViews>
   <sheets>
     <sheet name="companymasters" sheetId="1" r:id="rId1"/>
     <sheet name="departmentmasters" sheetId="2" r:id="rId2"/>
     <sheet name="designationmasters" sheetId="3" r:id="rId3"/>
+    <sheet name="citysubcitymasters" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>For testing</t>
   </si>
@@ -71,6 +76,21 @@
   </si>
   <si>
     <t>Auditor</t>
+  </si>
+  <si>
+    <t>CC0901</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>SCC7887</t>
+  </si>
+  <si>
+    <t>Tokyo</t>
+  </si>
+  <si>
+    <t>New Japan</t>
   </si>
 </sst>
 </file>
@@ -502,13 +522,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" customWidth="1"/>
-    <col min="5" max="5" width="37.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+    <col min="5" max="5" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -538,12 +558,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1">
+    <row r="4" spans="1:5" ht="15" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1">
+    <row r="5" spans="1:5" ht="15" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -567,12 +587,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" customWidth="1"/>
-    <col min="4" max="5" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="31.109375" customWidth="1"/>
+    <col min="4" max="5" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -612,13 +632,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E2DA2B4-0388-423D-8038-419F48C8B173}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
@@ -647,4 +667,43 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDA9DE4-C19C-49CE-8F0A-839098395501}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>